<commit_message>
varied the initial condition to test the relay-breaker combination. - Noticed problems when starting the breaker initially open
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,13 +905,13 @@
         <v>13800</v>
       </c>
       <c r="C3" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" s="8">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="F3" s="8">
         <v>0.5</v>
@@ -988,7 +988,7 @@
         <v>600</v>
       </c>
       <c r="H4" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7">
         <v>20</v>

</xml_diff>

<commit_message>
testing cb and relay models. also testing coordination between relays - issues found during faults and cb initial conitions.  the cb unit test proved the cb to operate correctly, next will test the relay
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>600</v>
       </c>
       <c r="H4" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7">
         <v>20</v>

</xml_diff>

<commit_message>
testing initial conditions - issues with relay response
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>600</v>
       </c>
       <c r="H4" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="7">
         <v>20</v>

</xml_diff>

<commit_message>
testing relay operation to multiple settings depending on fault current availability
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
+++ b/DistributionSystems/SimulinkOpal/Relay_Test/relay_settings/relay_parameters.xlsx
@@ -68,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -165,6 +178,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -735,7 +754,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="P17" sqref="P16:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +868,7 @@
         <v>0.5</v>
       </c>
       <c r="G2" s="7">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -861,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="7">
-        <v>0.6</v>
+        <v>13</v>
       </c>
       <c r="L2" s="7">
         <v>1</v>
@@ -869,10 +888,10 @@
       <c r="M2" s="7">
         <v>1</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="12">
         <v>0.9</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="12">
         <v>1.1000000000000001</v>
       </c>
       <c r="P2" s="7">
@@ -917,7 +936,7 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="7">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -929,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="7">
-        <v>0.6</v>
+        <v>10</v>
       </c>
       <c r="L3" s="7">
         <v>1</v>
@@ -937,10 +956,10 @@
       <c r="M3" s="7">
         <v>1</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="12">
         <v>0.9</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="12">
         <v>1.1000000000000001</v>
       </c>
       <c r="P3" s="7">
@@ -988,7 +1007,7 @@
         <v>600</v>
       </c>
       <c r="H4" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7">
         <v>20</v>
@@ -997,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="7">
-        <v>0.6</v>
+        <v>32</v>
       </c>
       <c r="L4" s="7">
         <v>1</v>
@@ -1005,10 +1024,10 @@
       <c r="M4" s="7">
         <v>1</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="12">
         <v>0.9</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="12">
         <v>1.1000000000000001</v>
       </c>
       <c r="P4" s="7">
@@ -1039,6 +1058,8 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>

</xml_diff>